<commit_message>
update Dart_Expert_Dow_6month.xlsx file name and add to data page
</commit_message>
<xml_diff>
--- a/docs/Data/Biggest_Loser.xlsx
+++ b/docs/Data/Biggest_Loser.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://webmailbyui-my.sharepoint.com/personal/drp36_byui_edu/Documents/221/Course_Files/BYUI_M221_Book/docs/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://webmailbyui-my.sharepoint.com/personal/drp36_byui_edu/Documents/221/Course_Files/BYUI_M221_Book/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61E5F3F6-DDC9-44E4-9B7E-23FB94573FFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEFC8335-E8FB-47B4-89A0-63E577B6C38D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8580" yWindow="1320" windowWidth="19875" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>